<commit_message>
Plowright family tree: v1.0.1
</commit_message>
<xml_diff>
--- a/families/plowright/xlsx/plowright_data_cleaned.xlsx
+++ b/families/plowright/xlsx/plowright_data_cleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\personal\family_trees\families\plowright\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943ED427-EED4-4B72-A742-37C632CB0A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE563D1B-9D5D-4521-8400-0442666FB57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2715" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individuals" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="557">
   <si>
     <t>Henry</t>
   </si>
@@ -1690,6 +1690,9 @@
   </si>
   <si>
     <t>Emil P.</t>
+  </si>
+  <si>
+    <t>Malin</t>
   </si>
 </sst>
 </file>
@@ -2245,8 +2248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0E20A4-86BC-4753-8113-72D57413D6B4}">
   <dimension ref="A1:X191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="237" workbookViewId="0">
-      <selection activeCell="N87" sqref="N87"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="237" workbookViewId="0">
+      <selection activeCell="L154" sqref="L154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6844,7 +6847,7 @@
         <v>282</v>
       </c>
       <c r="L154">
-        <v>1940</v>
+        <v>1943</v>
       </c>
       <c r="N154">
         <v>2011</v>
@@ -7192,6 +7195,9 @@
       <c r="E172" t="s">
         <v>34</v>
       </c>
+      <c r="F172" t="s">
+        <v>556</v>
+      </c>
       <c r="O172" t="s">
         <v>539</v>
       </c>
@@ -7294,9 +7300,6 @@
       </c>
       <c r="J175" t="s">
         <v>291</v>
-      </c>
-      <c r="K175" t="s">
-        <v>305</v>
       </c>
       <c r="L175">
         <v>1967</v>

</xml_diff>